<commit_message>
Add a few buildups to the model
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarem\Desktop\data_science\Data-Science-Projects\PO_PW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarem\Desktop\data_science\EE_lab\forecast_eastern_poland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D0F5B6-B2CC-43A2-AE24-AD2852BCACD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD84342-F691-4D80-BA1D-03073A53D61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22E14BC7-045F-4399-90F7-DACAEE225567}"/>
+    <workbookView xWindow="7305" yWindow="2085" windowWidth="13455" windowHeight="15405" xr2:uid="{22E14BC7-045F-4399-90F7-DACAEE225567}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +123,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,17 +150,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,10 +479,13 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -563,7 +580,7 @@
       <c r="I2" s="2">
         <v>1712</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="5">
         <v>74417.5</v>
       </c>
       <c r="K2" s="2">
@@ -628,7 +645,7 @@
       <c r="I3" s="2">
         <v>1550</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="5">
         <v>74535.099999999991</v>
       </c>
       <c r="K3" s="2">
@@ -693,8 +710,8 @@
       <c r="I4" s="2">
         <v>1941</v>
       </c>
-      <c r="J4" s="2">
-        <v>84242680</v>
+      <c r="J4" s="5">
+        <v>84242.68</v>
       </c>
       <c r="K4" s="2">
         <v>262358754</v>
@@ -758,7 +775,7 @@
       <c r="I5" s="2">
         <v>1806</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="5">
         <v>88850</v>
       </c>
       <c r="K5" s="2">
@@ -823,7 +840,7 @@
       <c r="I6" s="2">
         <v>1658</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="5">
         <v>86966.5</v>
       </c>
       <c r="K6" s="2">

</xml_diff>